<commit_message>
Some changes in BondRates Bot
</commit_message>
<xml_diff>
--- a/VNA/VNA.xlsx
+++ b/VNA/VNA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>VNA NTN-B</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>04/02/2022</t>
+  </si>
+  <si>
+    <t>07/02/2022</t>
   </si>
 </sst>
 </file>
@@ -392,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -449,6 +452,23 @@
         <v>9.15</v>
       </c>
     </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>3805.269454</v>
+      </c>
+      <c r="C4">
+        <v>11335.950417</v>
+      </c>
+      <c r="D4">
+        <v>0.55</v>
+      </c>
+      <c r="E4">
+        <v>10.65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
after that i will take the 'indicative rate'
</commit_message>
<xml_diff>
--- a/VNA/VNA.xlsx
+++ b/VNA/VNA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>VNA NTN-B</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>07/02/2022</t>
+  </si>
+  <si>
+    <t>08/02/2022</t>
+  </si>
+  <si>
+    <t>09/02/2022</t>
   </si>
 </sst>
 </file>
@@ -395,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -469,6 +475,40 @@
         <v>10.65</v>
       </c>
     </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>3806.263471</v>
+      </c>
+      <c r="C5">
+        <v>11340.503841</v>
+      </c>
+      <c r="D5">
+        <v>0.55</v>
+      </c>
+      <c r="E5">
+        <v>10.65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>3806.952118</v>
+      </c>
+      <c r="C6">
+        <v>11345.059095</v>
+      </c>
+      <c r="D6">
+        <v>0.54</v>
+      </c>
+      <c r="E6">
+        <v>10.65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
With operation buy/liquidate, and some comments about old functions
</commit_message>
<xml_diff>
--- a/VNA/VNA.xlsx
+++ b/VNA/VNA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>VNA NTN-B</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>09/02/2022</t>
+  </si>
+  <si>
+    <t>10/02/2022</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -509,6 +512,23 @@
         <v>10.65</v>
       </c>
     </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>3807.928593</v>
+      </c>
+      <c r="C7">
+        <v>11349.616178</v>
+      </c>
+      <c r="D7">
+        <v>0.54</v>
+      </c>
+      <c r="E7">
+        <v>10.65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>